<commit_message>
[Abraham]:fixed select all in enterprise.
</commit_message>
<xml_diff>
--- a/src/assets/anexos/creditos_preaprobados_automotriz_digital_ifis.xlsx
+++ b/src/assets/anexos/creditos_preaprobados_automotriz_digital_ifis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamactwo/Desktop/Project/BigPuntos/Front/coop-ifi-front-center/src/assets/anexos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92079E8-7B9B-CE49-A372-F80924EFA194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1DD7B3-26CE-5749-AFBE-EA2BA9DEE735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,9 +124,6 @@
     <t>1002003004003</t>
   </si>
   <si>
-    <t>1002003004001,1002003004002</t>
-  </si>
-  <si>
     <t>Jimmy</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
   </si>
   <si>
     <t>Cooperativa de Ahorro y Crédito San José de Vittoria</t>
+  </si>
+  <si>
+    <t>[1002003004001,1002003004002]</t>
   </si>
 </sst>
 </file>
@@ -227,7 +227,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -253,6 +253,7 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1417,7 +1418,7 @@
   <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1556,7 +1557,7 @@
         <v>31</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>32</v>
@@ -1569,10 +1570,10 @@
         <v>33</v>
       </c>
       <c r="V2" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" s="13" t="s">
         <v>39</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1604,7 +1605,7 @@
         <v>1003150602</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>27</v>
@@ -1625,23 +1626,23 @@
         <v>31</v>
       </c>
       <c r="Q3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="S3" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T3" s="8"/>
       <c r="U3" s="2" t="s">
         <v>33</v>
       </c>
       <c r="V3" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="W3" s="13" t="s">
         <v>39</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>